<commit_message>
Utworzenie procedury dodajKlienta. Zmiana ustawień kolumny dataAktywacji na nullable. Update readme i dokumentacji
</commit_message>
<xml_diff>
--- a/Dokumentacja/Opis tabel.xlsx
+++ b/Dokumentacja/Opis tabel.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remig\OneDrive\Pulpit\Asia GIT\Dokumentacja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remig\OneDrive\Pulpit\Asia GIT\Ksiegarnia.Database\Dokumentacja\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="OpisTabel" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="143">
   <si>
     <t>Kolumna(typ)</t>
   </si>
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1754,9 +1754,6 @@
       <c r="B62" t="s">
         <v>83</v>
       </c>
-      <c r="F62" t="s">
-        <v>20</v>
-      </c>
       <c r="G62" t="s">
         <v>105</v>
       </c>

</xml_diff>